<commit_message>
creating add product page with external data
</commit_message>
<xml_diff>
--- a/src/test/java/Utils_loc/data.xlsx
+++ b/src/test/java/Utils_loc/data.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Product_info" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -103,6 +103,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -294,10 +295,10 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.21"/>

</xml_diff>

<commit_message>
creating add product with external data
</commit_message>
<xml_diff>
--- a/src/test/java/Utils_loc/data.xlsx
+++ b/src/test/java/Utils_loc/data.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Categories</t>
   </si>
   <si>
-    <t xml:space="preserve">Electronics-others</t>
+    <t xml:space="preserve">Electronics &gt;&gt; Others</t>
   </si>
   <si>
     <t xml:space="preserve">Prices</t>
@@ -294,11 +294,11 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.21"/>

</xml_diff>

<commit_message>
Setup in progress for add products Page
</commit_message>
<xml_diff>
--- a/src/test/java/Utils_loc/data.xlsx
+++ b/src/test/java/Utils_loc/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Product Name</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Prices</t>
   </si>
   <si>
+    <t xml:space="preserve">600</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tax exempt</t>
   </si>
   <si>
@@ -76,19 +79,31 @@
     <t xml:space="preserve">weight</t>
   </si>
   <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
     <t xml:space="preserve">length</t>
   </si>
   <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
     <t xml:space="preserve">width</t>
   </si>
   <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
     <t xml:space="preserve">height</t>
   </si>
   <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inventory method</t>
   </si>
   <si>
-    <t xml:space="preserve">Don’t track inventory</t>
+    <t xml:space="preserve">Don't track inventory</t>
   </si>
 </sst>
 </file>
@@ -295,10 +310,10 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.21"/>
@@ -348,72 +363,72 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>600</v>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="n">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="n">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>